<commit_message>
Attendance Compoff/Overtime and Reports Updated.
</commit_message>
<xml_diff>
--- a/attendance/src/main/resources/TestData/Attendancepage.xlsx
+++ b/attendance/src/main/resources/TestData/Attendancepage.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EF7161A-CAE7-4159-8BFE-A9B7590AB0AD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF087F86-1169-438D-8DBA-7F973FB97A0A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="40">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -71,9 +71,6 @@
     <t>verify recorded clock in</t>
   </si>
   <si>
-    <t>Recorded Clock In</t>
-  </si>
-  <si>
     <t>verify final duration</t>
   </si>
   <si>
@@ -95,9 +92,6 @@
     <t>verify recorded clock out</t>
   </si>
   <si>
-    <t>Recorded Clock Out</t>
-  </si>
-  <si>
     <t>Policies display check</t>
   </si>
   <si>
@@ -141,6 +135,12 @@
   </si>
   <si>
     <t>Recorded Clock Out, when display of header is hidden</t>
+  </si>
+  <si>
+    <t>Time In</t>
+  </si>
+  <si>
+    <t>Time Out</t>
   </si>
 </sst>
 </file>
@@ -183,14 +183,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -471,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -484,6 +483,7 @@
     <col min="3" max="3" width="16.5546875" customWidth="1"/>
     <col min="4" max="4" width="16.88671875" customWidth="1"/>
     <col min="5" max="5" width="21.88671875" customWidth="1"/>
+    <col min="6" max="6" width="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -507,8 +507,8 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
-        <v>29</v>
+      <c r="A2" t="s">
+        <v>27</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>6</v>
@@ -527,14 +527,14 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>26</v>
+      <c r="A3" t="s">
+        <v>27</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
         <v>12</v>
@@ -546,248 +546,529 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>30</v>
       </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="B16" t="s">
         <v>16</v>
       </c>
-      <c r="F6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="C16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" t="s">
         <v>16</v>
       </c>
-      <c r="F7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
+      <c r="C17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>32</v>
       </c>
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="3" t="s">
+      <c r="B18" t="s">
         <v>18</v>
       </c>
-      <c r="F8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+      <c r="C18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="3" t="s">
+      <c r="B20" t="s">
         <v>18</v>
       </c>
-      <c r="F9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
+      <c r="C20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" t="s">
+        <v>19</v>
+      </c>
+      <c r="F20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" t="s">
+        <v>19</v>
+      </c>
+      <c r="F21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>34</v>
       </c>
-      <c r="B10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="B22" t="s">
         <v>20</v>
       </c>
-      <c r="F10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+      <c r="C22" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" t="s">
+        <v>21</v>
+      </c>
+      <c r="F22" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" t="s">
+        <v>21</v>
+      </c>
+      <c r="F23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="B24" t="s">
         <v>20</v>
       </c>
-      <c r="F11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
+      <c r="C24" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" t="s">
+        <v>21</v>
+      </c>
+      <c r="F24" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" t="s">
+        <v>12</v>
+      </c>
+      <c r="E25" t="s">
+        <v>21</v>
+      </c>
+      <c r="F25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>36</v>
       </c>
-      <c r="B12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="B26" t="s">
         <v>22</v>
       </c>
-      <c r="F12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+      <c r="C26" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" t="s">
+        <v>39</v>
+      </c>
+      <c r="F26" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" t="s">
+        <v>39</v>
+      </c>
+      <c r="F27" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="B28" t="s">
         <v>22</v>
       </c>
-      <c r="F13" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" t="s">
-        <v>24</v>
-      </c>
-      <c r="F14" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
+      <c r="C28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28" t="s">
         <v>39</v>
       </c>
-      <c r="B15" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15" t="s">
-        <v>24</v>
-      </c>
-      <c r="F15" t="s">
+      <c r="F28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B29" t="s">
+        <v>22</v>
+      </c>
+      <c r="C29" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" t="s">
+        <v>12</v>
+      </c>
+      <c r="E29" t="s">
+        <v>39</v>
+      </c>
+      <c r="F29" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -796,7 +1077,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -826,10 +1107,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>

</xml_diff>